<commit_message>
adicionado inicio da funcao de compartilhar imagem
</commit_message>
<xml_diff>
--- a/shareResources/tabela.xlsx
+++ b/shareResources/tabela.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Documentos\boloscar\shareResources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c464348844b5e98/Documentos/boloscar/shareResources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79938DA6-5A4B-420C-AC25-E896042CEB58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{79938DA6-5A4B-420C-AC25-E896042CEB58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{19B55236-A9EF-43F8-AC64-FEFA5E846323}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B61F925C-DC8F-4177-B0CE-FC10AE9CF03D}"/>
+    <workbookView xWindow="3120" yWindow="600" windowWidth="19200" windowHeight="15600" xr2:uid="{B61F925C-DC8F-4177-B0CE-FC10AE9CF03D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="72">
   <si>
     <t>Categoria</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>Coringa</t>
-  </si>
-  <si>
-    <t>The neighbors' Window</t>
   </si>
   <si>
     <t>Hair Love</t>
@@ -208,12 +205,93 @@
       <t>❌</t>
     </r>
   </si>
+  <si>
+    <t>The neighbors Window</t>
+  </si>
+  <si>
+    <t>catFilme</t>
+  </si>
+  <si>
+    <t>char(255)</t>
+  </si>
+  <si>
+    <t>catDirecao</t>
+  </si>
+  <si>
+    <t>catFotografia</t>
+  </si>
+  <si>
+    <t>catArte</t>
+  </si>
+  <si>
+    <t>catrotAdapt</t>
+  </si>
+  <si>
+    <t>catrotOrig</t>
+  </si>
+  <si>
+    <t>catAtriz</t>
+  </si>
+  <si>
+    <t>catAtor</t>
+  </si>
+  <si>
+    <t>catAtrizCoad</t>
+  </si>
+  <si>
+    <t>catAtorCoad</t>
+  </si>
+  <si>
+    <t>catEfeitos</t>
+  </si>
+  <si>
+    <t>catEdicao</t>
+  </si>
+  <si>
+    <t>catAnimacao</t>
+  </si>
+  <si>
+    <t>catEstrangeiro</t>
+  </si>
+  <si>
+    <t>catMixSom</t>
+  </si>
+  <si>
+    <t>catEdiSom</t>
+  </si>
+  <si>
+    <t>catFigurino</t>
+  </si>
+  <si>
+    <t>catMaquiagem</t>
+  </si>
+  <si>
+    <t>catDocumentario</t>
+  </si>
+  <si>
+    <t>catTrilha</t>
+  </si>
+  <si>
+    <t>catCurta</t>
+  </si>
+  <si>
+    <t>catMusica</t>
+  </si>
+  <si>
+    <t>catAnimacaoCurta</t>
+  </si>
+  <si>
+    <t>catDocCurta</t>
+  </si>
+  <si>
+    <t>Pontuação total:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +340,34 @@
       <sz val="24"/>
       <color rgb="FFAB8307"/>
       <name val="Serifa"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF717171"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -343,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -365,6 +471,27 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -687,24 +814,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF964412-713F-44AC-B89E-5D855814F624}">
-  <dimension ref="B3:J27"/>
+  <dimension ref="B2:M60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="44" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
-    <col min="5" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="54.7109375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="28.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="32.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="34.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="54.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="35.25" customHeight="1" thickBot="1">
+    <row r="2" spans="2:13">
+      <c r="C2" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="35.25" customHeight="1" thickBot="1">
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -712,40 +851,67 @@
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="19.5" thickTop="1">
+        <v>44</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="23.25" thickTop="1">
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="str">
-        <f>IF(LEN(J4)&gt;25,LEFT(J4,22)&amp;"...",J4)</f>
+        <f>IF(LEN(M4)&gt;25,LEFT(M4,22)&amp;"...",M4)</f>
         <v>Parasita</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="18.75">
+    <row r="5" spans="2:13" ht="22.5">
       <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="5" t="str">
-        <f t="shared" ref="C5:C27" si="0">IF(LEN(J5)&gt;25,LEFT(J5,22)&amp;"...",J5)</f>
+        <f t="shared" ref="C5:C27" si="0">IF(LEN(M5)&gt;25,LEFT(M5,22)&amp;"...",M5)</f>
         <v>Bong Joon Ho - Parasita</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="F5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="18.75">
+    <row r="6" spans="2:13" ht="22.5">
       <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
@@ -756,11 +922,20 @@
       <c r="D6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="3">
+      <c r="F6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="3">
         <v>1917</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="18.75">
+    <row r="7" spans="2:13" ht="22.5">
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
@@ -771,11 +946,20 @@
       <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="F7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="18.75">
+    <row r="8" spans="2:13" ht="22.5">
       <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
@@ -786,11 +970,20 @@
       <c r="D8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="F8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="18.75">
+    <row r="9" spans="2:13" ht="22.5">
       <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
@@ -801,11 +994,20 @@
       <c r="D9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="F9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="18.75">
+    <row r="10" spans="2:13" ht="22.5">
       <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
@@ -816,11 +1018,20 @@
       <c r="D10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="F10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="18.75">
+    <row r="11" spans="2:13" ht="22.5">
       <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
@@ -831,11 +1042,20 @@
       <c r="D11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="F11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="18.75">
+    <row r="12" spans="2:13" ht="22.5">
       <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
@@ -846,11 +1066,20 @@
       <c r="D12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="F12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="18.75">
+    <row r="13" spans="2:13" ht="22.5">
       <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
@@ -861,11 +1090,20 @@
       <c r="D13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="F13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="18.75">
+    <row r="14" spans="2:13" ht="22.5">
       <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
@@ -876,11 +1114,20 @@
       <c r="D14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="3">
+      <c r="F14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="3">
         <v>1917</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="18.75">
+    <row r="15" spans="2:13" ht="22.5">
       <c r="B15" s="7" t="s">
         <v>13</v>
       </c>
@@ -891,11 +1138,20 @@
       <c r="D15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="F15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="18.75">
+    <row r="16" spans="2:13" ht="22.5">
       <c r="B16" s="7" t="s">
         <v>14</v>
       </c>
@@ -906,11 +1162,20 @@
       <c r="D16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="F16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="18.75">
+    <row r="17" spans="2:13" ht="22.5">
       <c r="B17" s="7" t="s">
         <v>15</v>
       </c>
@@ -921,11 +1186,20 @@
       <c r="D17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="F17" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="18.75">
+    <row r="18" spans="2:13" ht="22.5">
       <c r="B18" s="7" t="s">
         <v>16</v>
       </c>
@@ -936,11 +1210,20 @@
       <c r="D18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="3">
+      <c r="F18" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="3">
         <v>1917</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="18.75">
+    <row r="19" spans="2:13" ht="22.5">
       <c r="B19" s="7" t="s">
         <v>17</v>
       </c>
@@ -951,11 +1234,20 @@
       <c r="D19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="F19" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="18.75">
+    <row r="20" spans="2:13" ht="22.5">
       <c r="B20" s="7" t="s">
         <v>18</v>
       </c>
@@ -966,11 +1258,20 @@
       <c r="D20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="F20" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="18.75">
+    <row r="21" spans="2:13" ht="22.5">
       <c r="B21" s="7" t="s">
         <v>19</v>
       </c>
@@ -981,11 +1282,20 @@
       <c r="D21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="F21" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="18.75">
+    <row r="22" spans="2:13" ht="22.5">
       <c r="B22" s="7" t="s">
         <v>20</v>
       </c>
@@ -996,11 +1306,20 @@
       <c r="D22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="F22" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="18.75">
+    <row r="23" spans="2:13" ht="22.5">
       <c r="B23" s="7" t="s">
         <v>21</v>
       </c>
@@ -1011,26 +1330,44 @@
       <c r="D23" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="F23" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M23" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="18.75">
+    <row r="24" spans="2:13" ht="22.5">
       <c r="B24" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>The neighbors' Window</v>
+        <v>The neighbors Window</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="18.75">
+      <c r="F24" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" ht="22.5">
       <c r="B25" s="7" t="s">
         <v>23</v>
       </c>
@@ -1041,11 +1378,20 @@
       <c r="D25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J25" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" ht="18.75">
+      <c r="F25" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="22.5">
       <c r="B26" s="7" t="s">
         <v>24</v>
       </c>
@@ -1056,11 +1402,20 @@
       <c r="D26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" ht="18.75">
+      <c r="F26" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" ht="22.5">
       <c r="B27" s="7" t="s">
         <v>25</v>
       </c>
@@ -1071,8 +1426,361 @@
       <c r="D27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>43</v>
+      <c r="F27" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13">
+      <c r="F32" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8">
+      <c r="C37" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8">
+      <c r="C38" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8">
+      <c r="C39" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8">
+      <c r="C40" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8">
+      <c r="C41" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8">
+      <c r="C42" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8">
+      <c r="C43" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8">
+      <c r="C44" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8">
+      <c r="C45" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8">
+      <c r="C46" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H46" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8">
+      <c r="C47" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8">
+      <c r="C48" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8">
+      <c r="C49" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H49" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8">
+      <c r="C50" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8">
+      <c r="C51" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8">
+      <c r="C52" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8">
+      <c r="C53" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8">
+      <c r="C54" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8">
+      <c r="C55" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H55" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8">
+      <c r="C56" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8">
+      <c r="C57" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8">
+      <c r="C58" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8">
+      <c r="C59" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8">
+      <c r="C60" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>